<commit_message>
translated symptoms and diseases to french
</commit_message>
<xml_diff>
--- a/datasets/cat_dog_dataset.xlsx
+++ b/datasets/cat_dog_dataset.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhadjarab/pa/tonveto/ai_back/datasets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE2C2BF-92ED-3147-9F3F-508D9DB48E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$A$10</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -25,69 +34,67 @@
     <t>Symptoms</t>
   </si>
   <si>
-    <t>dog/cat</t>
-  </si>
-  <si>
-    <t>KIDNEY DISEASE</t>
-  </si>
-  <si>
-    <t>Frequent urination, Weight loss, Drinking a lot of water, dry coat, Vomiting, Diarrhea, Bloody or cloudy urine</t>
-  </si>
-  <si>
-    <t>DIABETES</t>
-  </si>
-  <si>
-    <t>Weight loss, Increased thirst and/or urination, Lethargy, Dehydration, Change in appetite, Sweet-smelling breath</t>
-  </si>
-  <si>
-    <t>FELINE IMMUNODEFICIENCY VIRUS (FIV)</t>
-  </si>
-  <si>
-    <t>Gingivitis, Loss of appetite, Poor coat condition, Fever, Chronic or recurring infections</t>
-  </si>
-  <si>
-    <t>FELINE LEUKEMIA VIRUS (FELV)</t>
-  </si>
-  <si>
-    <t>Seizures or neurological disorders, Various eye conditions, Persistent diarrhea, Persistent fever, Skin, urinary or respiratory infections, Weight loss, Loss of appetite</t>
-  </si>
-  <si>
     <t>CANCER</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight loss, Anorexia, Diarrhea, Vomiting, Swelling, Lumps, skin infections, bad breath
-</t>
-  </si>
-  <si>
-    <t>PANCREATITIS</t>
-  </si>
-  <si>
-    <t>Vomiting, Fever, Abdominal pain, Decreased appetite, Diarrhea</t>
-  </si>
-  <si>
-    <t>HYPERTHYROIDISM</t>
-  </si>
-  <si>
-    <t>Excessive amounts of energy, Increased appetite,Weight loss, Restlessness</t>
-  </si>
-  <si>
-    <t>Heartworm</t>
-  </si>
-  <si>
-    <t>Labored breathing, Coughing, Vomiting, Weight loss, listlessness and fatigue after only moderate exercise</t>
-  </si>
-  <si>
-    <t>Rabies</t>
-  </si>
-  <si>
-    <t>Attacking other animals, humans and even inanimate objects, Licking, biting and chewing at the bite site, Fever, Hypersensitivity, Hiding in dark places, Eating unusual objects, Paralysis of the throat and jaw muscles, Foaming at the mouth, Disorientation, incoordination and staggering, Paralysis of the hind legs, Loss of appetite, Weakness, Seizures, Sudden death</t>
+    <t>chat/chien</t>
+  </si>
+  <si>
+    <t>MALADIE DU REIN</t>
+  </si>
+  <si>
+    <t>DIABÈTE</t>
+  </si>
+  <si>
+    <t>VIRUS DE L'IMMUNODÉFICIENCE FÉLINE (FIV)</t>
+  </si>
+  <si>
+    <t>VIRUS DE LA LEUCÉMIE FÉLINE (FELV)</t>
+  </si>
+  <si>
+    <t>PANCRÉATITE</t>
+  </si>
+  <si>
+    <t>HYPERTHYROÏDIE</t>
+  </si>
+  <si>
+    <t>Dirofilariose</t>
+  </si>
+  <si>
+    <t>Rage</t>
+  </si>
+  <si>
+    <t>Besoin fréquent d'uriner, perte de poids, boire beaucoup d'eau, pelage sec, vomissements, diarrhée, urine sanglante ou trouble</t>
+  </si>
+  <si>
+    <t>Weight loss, Increased thirst and/or urination, Lethargy, Dehydration, Change in appetite, Sweet-smelling brePerte de poids, augmentation de la soif et/ou de la miction, léthargie, déshydratation, modification de l'appétit, haleine odorante</t>
+  </si>
+  <si>
+    <t>Gingivite, Perte d'appétit, Mauvais état du pelage, Fièvre, Infections chroniques ou récurrentes</t>
+  </si>
+  <si>
+    <t>Convulsions ou troubles neurologiques, Diverses affections oculaires, Diarrhée persistante, Fièvre persistante, Infections cutanées, urinaires ou respiratoires, Perte de poids, Perte d'appétit</t>
+  </si>
+  <si>
+    <t>Perte de poids, anorexie, diarrhée, vomissements, gonflement, grumeaux, infections cutanées, mauvaise haleine</t>
+  </si>
+  <si>
+    <t>Vomissements, Fièvre, Douleurs abdominales, Diminution de l'appétit, Diarrhée</t>
+  </si>
+  <si>
+    <t>Quantités excessives d'énergie, augmentation de l'appétit, perte de poids, agitation</t>
+  </si>
+  <si>
+    <t>Respiration laborieuse, toux, vomissements, perte de poids, apathie et fatigue après seulement un exercice modéré</t>
+  </si>
+  <si>
+    <t>Attaquer d'autres animaux et humains et même des objets inanimés, Lécher, mordre et mâcher à l'endroit de la morsure, Fièvre, Hypersensibilité, Se cacher dans des endroits sombres, Manger des objets inhabituels, Paralysie de la gorge et des muscles de la mâchoire, Mousse à la bouche, Désorientation, incoordination et chancelante, paralysie des pattes postérieures, perte d'appétit, faiblesse, convulsions, mort subite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,26 +145,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -168,10 +175,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -209,71 +216,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -301,7 +308,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -324,11 +331,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -337,13 +344,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -353,7 +360,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -362,7 +369,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -371,7 +378,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -379,10 +386,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -447,22 +454,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,106 +483,107 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:A10" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>